<commit_message>
Basic support to MySQL and MariaDB. Several other improvements.
</commit_message>
<xml_diff>
--- a/support_matrix.xlsx
+++ b/support_matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34">
   <si>
     <t>OmniDB</t>
   </si>
@@ -105,9 +105,6 @@
     <t>MySQL</t>
   </si>
   <si>
-    <t>5.5.x</t>
-  </si>
-  <si>
     <t>5.6.x</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
   </si>
   <si>
     <t>MariaDB</t>
-  </si>
-  <si>
-    <t>10.0.x</t>
   </si>
   <si>
     <t>10.1.x</t>
@@ -132,11 +126,18 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,7 +156,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,7 +170,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,11 +230,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -208,82 +284,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -298,6 +299,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -310,180 +329,162 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="24">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -624,27 +625,59 @@
       <left style="medium">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -693,6 +726,21 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -714,6 +762,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -729,6 +801,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -747,58 +845,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -807,152 +855,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -986,22 +1034,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1319,10 +1382,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="B2:L26"/>
+  <dimension ref="B2:L23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1382,7 +1445,7 @@
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -1413,7 +1476,7 @@
       <c r="D6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
@@ -1444,7 +1507,7 @@
       <c r="D7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1475,7 +1538,7 @@
       <c r="D8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="6" t="s">
@@ -1506,7 +1569,7 @@
       <c r="D9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="6" t="s">
@@ -1537,7 +1600,7 @@
       <c r="D10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="15"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="6" t="s">
         <v>12</v>
       </c>
@@ -1568,7 +1631,7 @@
       <c r="D11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="15"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6" t="s">
         <v>12</v>
@@ -1597,7 +1660,7 @@
       <c r="D12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="15"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="6" t="s">
         <v>12</v>
       </c>
@@ -1626,7 +1689,7 @@
       <c r="D13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="15"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="6" t="s">
         <v>12</v>
       </c>
@@ -1657,7 +1720,7 @@
       <c r="D14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
         <v>12</v>
@@ -1684,7 +1747,7 @@
       <c r="D15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="15"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6" t="s">
         <v>12</v>
@@ -1711,7 +1774,7 @@
       <c r="D16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="15"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
         <v>12</v>
@@ -1740,7 +1803,7 @@
       <c r="D17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="15"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -1761,7 +1824,7 @@
       <c r="D18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="15"/>
+      <c r="E18" s="19"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -1782,7 +1845,7 @@
       <c r="D19" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="15"/>
+      <c r="E19" s="19"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1798,14 +1861,14 @@
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" spans="2:12">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="15"/>
+      <c r="E20" s="19"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -1817,12 +1880,12 @@
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" spans="2:12">
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7" t="s">
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="15"/>
+      <c r="E21" s="19"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -1834,12 +1897,14 @@
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" spans="2:12">
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10" t="s">
+      <c r="B22" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="15"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="19"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -1851,72 +1916,19 @@
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" spans="2:12">
-      <c r="B23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" ht="15" customHeight="1" spans="2:12">
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7" t="s">
+      <c r="B23" s="15"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" ht="15" customHeight="1" spans="2:12">
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" ht="15" customHeight="1" spans="2:12">
-      <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="13" t="s">
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="17" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1928,8 +1940,8 @@
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="B17:C19"/>
-    <mergeCell ref="B20:C22"/>
-    <mergeCell ref="B23:C26"/>
+    <mergeCell ref="B20:C21"/>
+    <mergeCell ref="B22:C23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Removed BDR support from core
</commit_message>
<xml_diff>
--- a/support_matrix.xlsx
+++ b/support_matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52">
   <si>
     <t>OmniDB</t>
   </si>
@@ -57,6 +57,9 @@
     <t>2.11.x</t>
   </si>
   <si>
+    <t>2.12.x</t>
+  </si>
+  <si>
     <t>PostgreSQL</t>
   </si>
   <si>
@@ -90,6 +93,9 @@
     <t>2.x</t>
   </si>
   <si>
+    <t>(1)</t>
+  </si>
+  <si>
     <t>3.x</t>
   </si>
   <si>
@@ -99,15 +105,21 @@
     <t>0.x</t>
   </si>
   <si>
+    <t>(2)</t>
+  </si>
+  <si>
     <t>1.x</t>
   </si>
   <si>
-    <t>(1)</t>
+    <t>(3)</t>
   </si>
   <si>
     <t>Postgres-XL</t>
   </si>
   <si>
+    <t>(4)</t>
+  </si>
+  <si>
     <t>Oracle</t>
   </si>
   <si>
@@ -138,13 +150,22 @@
     <t>10.2.x</t>
   </si>
   <si>
-    <t>(1) Support to BDR 3 was removed from core and converted to a plugin.</t>
+    <t>(1) Support to pglogical 2/3 was removed from core and converted to a plugin.</t>
+  </si>
+  <si>
+    <t>(2) Support to BDR 1/2 was removed from core and converted to a plugin.</t>
   </si>
   <si>
     <t>Not implemented yet</t>
   </si>
   <si>
+    <t>(3) Support to BDR 3 was removed from core and converted to a plugin.</t>
+  </si>
+  <si>
     <t>Supported in OmniDB core</t>
+  </si>
+  <si>
+    <t>(4) Support to Postgres-XL was removed from core and converted to a plugin.</t>
   </si>
   <si>
     <t>Supported in an external plugin</t>
@@ -158,8 +179,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -195,11 +216,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -219,24 +240,15 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,31 +262,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -286,8 +278,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -295,13 +302,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -316,12 +316,33 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -362,43 +383,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,133 +551,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -891,10 +912,10 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -904,10 +925,8 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -917,7 +936,9 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -928,7 +949,7 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -961,6 +982,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -971,36 +1022,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1011,6 +1032,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1023,155 +1055,144 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1194,39 +1215,33 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1263,10 +1278,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1329,43 +1347,46 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1683,10 +1704,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="B2:P33"/>
+  <dimension ref="B3:Q33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1695,553 +1716,603 @@
     <col min="2" max="2" width="11.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
-    <col min="5" max="14" width="6.625" style="2" customWidth="1"/>
-    <col min="15" max="16" width="6.625" style="3" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="1"/>
+    <col min="5" max="17" width="6.625" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="13.5"/>
-    <row r="3" ht="30" customHeight="1" spans="5:16">
-      <c r="E3" s="26" t="s">
+    <row r="3" ht="30" customHeight="1" spans="5:17">
+      <c r="E3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="48"/>
-    </row>
-    <row r="4" ht="15" customHeight="1" spans="5:16">
-      <c r="E4" s="28" t="s">
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="55"/>
+    </row>
+    <row r="4" ht="15" customHeight="1" spans="5:17">
+      <c r="E4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="29" t="s">
+      <c r="I4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="29" t="s">
+      <c r="L4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="29" t="s">
+      <c r="M4" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="49" t="s">
+      <c r="N4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="49" t="s">
+      <c r="O4" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="50" t="s">
+      <c r="P4" s="48" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" ht="15" customHeight="1" spans="2:16">
-      <c r="B5" s="4" t="s">
+      <c r="Q4" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5" t="s">
+    </row>
+    <row r="5" ht="15" customHeight="1" spans="2:17">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="53"/>
-    </row>
-    <row r="6" ht="15" customHeight="1" spans="2:16">
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9" t="s">
+      <c r="D5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="54"/>
-      <c r="P6" s="55"/>
-    </row>
-    <row r="7" ht="15" customHeight="1" spans="2:16">
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9" t="s">
+      <c r="E5" s="29"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="57"/>
+    </row>
+    <row r="6" ht="15" customHeight="1" spans="2:17">
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="55"/>
-    </row>
-    <row r="8" ht="15" customHeight="1" spans="2:16">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9" t="s">
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="50"/>
+    </row>
+    <row r="7" ht="15" customHeight="1" spans="2:17">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="54"/>
-      <c r="P8" s="55"/>
-    </row>
-    <row r="9" ht="15" customHeight="1" spans="2:16">
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9" t="s">
+      <c r="E7" s="31"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="58"/>
+    </row>
+    <row r="8" ht="15" customHeight="1" spans="2:17">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="54"/>
-      <c r="P9" s="55"/>
-    </row>
-    <row r="10" ht="15" customHeight="1" spans="2:16">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9" t="s">
+      <c r="E8" s="31"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="58"/>
+    </row>
+    <row r="9" ht="15" customHeight="1" spans="2:17">
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="54"/>
-      <c r="P10" s="55"/>
-    </row>
-    <row r="11" ht="15" customHeight="1" spans="2:16">
-      <c r="B11" s="7"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="9" t="s">
+      <c r="E9" s="31"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="58"/>
+    </row>
+    <row r="10" ht="15" customHeight="1" spans="2:17">
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="56"/>
-      <c r="O11" s="56"/>
-      <c r="P11" s="55"/>
-    </row>
-    <row r="12" ht="15" customHeight="1" spans="2:16">
-      <c r="B12" s="7"/>
-      <c r="C12" s="11" t="s">
+      <c r="E10" s="33"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="58"/>
+    </row>
+    <row r="11" ht="15" customHeight="1" spans="2:17">
+      <c r="B11" s="6"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="E11" s="33"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="58"/>
+    </row>
+    <row r="12" ht="15" customHeight="1" spans="2:17">
+      <c r="B12" s="6"/>
+      <c r="C12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="54"/>
-      <c r="P12" s="55"/>
-    </row>
-    <row r="13" ht="15" customHeight="1" spans="2:16">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="54"/>
-      <c r="O13" s="54"/>
-      <c r="P13" s="55"/>
-    </row>
-    <row r="14" ht="15" customHeight="1" spans="2:16">
-      <c r="B14" s="7"/>
-      <c r="C14" s="11" t="s">
+      <c r="E12" s="33"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="9" t="s">
+    </row>
+    <row r="13" ht="15" customHeight="1" spans="2:17">
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="34"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="55"/>
-    </row>
-    <row r="15" ht="15" customHeight="1" spans="2:16">
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9" t="s">
+      <c r="E13" s="33"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="53" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1" spans="2:17">
+      <c r="B14" s="6"/>
+      <c r="C14" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="54"/>
-      <c r="P15" s="55"/>
-    </row>
-    <row r="16" ht="15" customHeight="1" spans="2:16">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="54"/>
-      <c r="P16" s="55"/>
-    </row>
-    <row r="17" ht="15" customHeight="1" spans="2:16">
-      <c r="B17" s="7"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="9" t="s">
+      <c r="D14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="33"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="53" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1" spans="2:17">
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="33"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="53" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1" spans="2:17">
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="O17" s="57"/>
-      <c r="P17" s="58"/>
-    </row>
-    <row r="18" ht="15" customHeight="1" spans="2:16">
-      <c r="B18" s="7"/>
-      <c r="C18" s="12" t="s">
+      <c r="E16" s="33"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="34"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="55"/>
-    </row>
-    <row r="19" ht="15" customHeight="1" spans="2:16">
-      <c r="B19" s="7"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="9" t="s">
+    </row>
+    <row r="17" ht="15" customHeight="1" spans="2:17">
+      <c r="B17" s="6"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="33"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="O17" s="52"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="59"/>
+    </row>
+    <row r="18" ht="15" customHeight="1" spans="2:17">
+      <c r="B18" s="6"/>
+      <c r="C18" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="34"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="54"/>
-      <c r="O19" s="54"/>
-      <c r="P19" s="55"/>
-    </row>
-    <row r="20" ht="15" customHeight="1" spans="2:16">
-      <c r="B20" s="7"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14" t="s">
+      <c r="E18" s="33"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" ht="15" customHeight="1" spans="2:17">
+      <c r="B19" s="6"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="34"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="54"/>
-      <c r="O20" s="54"/>
-      <c r="P20" s="55"/>
-    </row>
-    <row r="21" ht="15" customHeight="1" spans="2:16">
-      <c r="B21" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="34"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="54"/>
-      <c r="O21" s="54"/>
-      <c r="P21" s="55"/>
-    </row>
-    <row r="22" ht="15" customHeight="1" spans="2:16">
-      <c r="B22" s="17"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="34"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="54"/>
-      <c r="O22" s="54"/>
-      <c r="P22" s="55"/>
-    </row>
-    <row r="23" ht="15" customHeight="1" spans="2:16">
-      <c r="B23" s="18"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14" t="s">
+      <c r="E19" s="33"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="34"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="55"/>
-    </row>
-    <row r="24" ht="15" customHeight="1" spans="2:16">
-      <c r="B24" s="19" t="s">
+    </row>
+    <row r="20" ht="15" customHeight="1" spans="2:17">
+      <c r="B20" s="6"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="33"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" ht="15" customHeight="1" spans="2:17">
+      <c r="B21" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="6" t="s">
+      <c r="C21" s="14"/>
+      <c r="D21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="34"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="54"/>
-      <c r="O24" s="54"/>
-      <c r="P24" s="55"/>
-    </row>
-    <row r="25" ht="15" customHeight="1" spans="2:16">
-      <c r="B25" s="21"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="14" t="s">
+      <c r="E21" s="33"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="51"/>
+      <c r="Q21" s="58"/>
+    </row>
+    <row r="22" ht="15" customHeight="1" spans="2:17">
+      <c r="B22" s="15"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="54"/>
-      <c r="P25" s="55"/>
-    </row>
-    <row r="26" ht="15" customHeight="1" spans="2:16">
-      <c r="B26" s="19" t="s">
+      <c r="E22" s="33"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="51"/>
+      <c r="Q22" s="58"/>
+    </row>
+    <row r="23" ht="15" customHeight="1" spans="2:17">
+      <c r="B23" s="16"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="6" t="s">
+      <c r="E23" s="33"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="58"/>
+    </row>
+    <row r="24" ht="15" customHeight="1" spans="2:17">
+      <c r="B24" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="54"/>
-      <c r="O26" s="54"/>
-      <c r="P26" s="55"/>
-    </row>
-    <row r="27" ht="15" customHeight="1" spans="2:16">
-      <c r="B27" s="23"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="25" t="s">
+      <c r="C24" s="18"/>
+      <c r="D24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="59"/>
-      <c r="O27" s="59"/>
-      <c r="P27" s="60"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="58"/>
+    </row>
+    <row r="25" ht="15" customHeight="1" spans="2:17">
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="33"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="58"/>
+    </row>
+    <row r="26" ht="15" customHeight="1" spans="2:17">
+      <c r="B26" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="33"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="58"/>
+    </row>
+    <row r="27" ht="15" customHeight="1" spans="2:17">
+      <c r="B27" s="21"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="35"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="54"/>
+      <c r="Q27" s="60"/>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="11:12">
-      <c r="K30" s="43"/>
-      <c r="L30" s="44" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="11:12">
-      <c r="K31" s="45"/>
-      <c r="L31" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="11:12">
-      <c r="K32" s="46"/>
-      <c r="L32" s="44" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12">
+      <c r="B30" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="K30" s="42"/>
+      <c r="L30" s="43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12">
+      <c r="B31" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="K31" s="44"/>
+      <c r="L31" s="43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12">
+      <c r="B32" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="K32" s="45"/>
+      <c r="L32" s="43" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="11:12">
-      <c r="K33" s="47"/>
-      <c r="L33" s="44" t="s">
-        <v>44</v>
+      <c r="K33" s="46"/>
+      <c r="L33" s="43" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="E3:P3"/>
+    <mergeCell ref="E3:Q3"/>
     <mergeCell ref="B5:B20"/>
     <mergeCell ref="C5:C11"/>
     <mergeCell ref="C12:C13"/>

</xml_diff>